<commit_message>
Eliminada la memoria en word
</commit_message>
<xml_diff>
--- a/documentación/Requisitos.xlsx
+++ b/documentación/Requisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UBU\TFG\TFG-ReservApp\documentación\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE6237F-596A-4ABF-9273-1F8E26559199}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82EC6FA0-1504-43B1-906F-85CDA431FD19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{99B74F84-E294-4824-9AE6-956FF75C7F75}"/>
   </bookViews>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Requisitos</t>
   </si>
   <si>
-    <t>El Usuario debe iniciar Sesión</t>
-  </si>
-  <si>
-    <t>El Usuario debe regitrarse</t>
-  </si>
-  <si>
     <t>RQ01</t>
   </si>
   <si>
@@ -77,52 +71,34 @@
     <t>RQ10</t>
   </si>
   <si>
-    <t>RQ11</t>
-  </si>
-  <si>
-    <t>RQ12</t>
-  </si>
-  <si>
-    <t>RQ13</t>
-  </si>
-  <si>
-    <t>RQ14</t>
-  </si>
-  <si>
-    <t>El Usuario podrá visualizar los Estbalecimientos asignados</t>
-  </si>
-  <si>
-    <t>El Administrador podrá gestionar Establecimientos</t>
-  </si>
-  <si>
-    <t>El Administrador podrá gestionar Usuarios</t>
-  </si>
-  <si>
-    <t>El Administrador podrá gestionar Reservas</t>
-  </si>
-  <si>
-    <t>El Administrador podrá gestionar Horarios de Establecimientos</t>
-  </si>
-  <si>
-    <t>El Usuario podrá consultar una Reserva</t>
-  </si>
-  <si>
-    <t>El Usuario podrá realizar una Reserva para un determinado Establecimiento</t>
-  </si>
-  <si>
-    <t>El Usuario podrá modificar una Reserva</t>
-  </si>
-  <si>
-    <t>El Usuario podrá anular una Reserva</t>
-  </si>
-  <si>
-    <t>El Usuario podrá consultar la disponibilidad de un Establecimiento</t>
-  </si>
-  <si>
-    <t>El Usuario podrá modificar su perfil</t>
-  </si>
-  <si>
-    <t>El Usuario podrá finalizar la Sesión</t>
+    <t>Gestión de Autenticación y Autorización</t>
+  </si>
+  <si>
+    <t>Registro de Usuarios</t>
+  </si>
+  <si>
+    <t>Gestión de Establecimientos</t>
+  </si>
+  <si>
+    <t>Sistema de Reservas</t>
+  </si>
+  <si>
+    <t>Sistema de Convocatorias</t>
+  </si>
+  <si>
+    <t>Búsqueda de Usuarios</t>
+  </si>
+  <si>
+    <t>Administración de Usuarios</t>
+  </si>
+  <si>
+    <t>Visualización de Reservas Administrativas</t>
+  </si>
+  <si>
+    <t>Gestión de Perfiles</t>
+  </si>
+  <si>
+    <t>Notificaciones por Email</t>
   </si>
 </sst>
 </file>
@@ -526,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE6F31BB-1F47-483D-844F-8F8D2BDEC48E}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A12" sqref="A12:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,113 +521,81 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>